<commit_message>
:beers: Datos de ejemplo
</commit_message>
<xml_diff>
--- a/document/datos.xlsx
+++ b/document/datos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t xml:space="preserve">Tipo Doc</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">EPS Y MEDICINA PREPAGADA SURAMERICANA S.A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI</t>
   </si>
 </sst>
 </file>
@@ -385,15 +388,17 @@
     <tabColor rgb="FFA9D18E"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -542,11 +547,59 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>144587410</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>44552</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
+  <conditionalFormatting sqref="B2:B4">
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>